<commit_message>
Part1 done for spain building
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,22 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA49EAE7-7B37-42B3-B706-19D5C4BE8BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286035AE-208A-4E8E-9C2C-2FFA586F27F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Settingsold" sheetId="1" r:id="rId1"/>
-    <sheet name="Settings" sheetId="4" r:id="rId2"/>
-    <sheet name="Constants" sheetId="2" r:id="rId3"/>
-    <sheet name="Assets" sheetId="3" r:id="rId4"/>
+    <sheet name="Settings" sheetId="4" r:id="rId1"/>
+    <sheet name="Constants" sheetId="2" r:id="rId2"/>
+    <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -49,15 +48,9 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>DirectorioClavesPath</t>
-  </si>
-  <si>
     <t>BlackListTrackingPath</t>
   </si>
   <si>
-    <t>TRADPath</t>
-  </si>
-  <si>
     <t>FTPport</t>
   </si>
   <si>
@@ -73,9 +66,6 @@
     <t>in_BlackListSheetName</t>
   </si>
   <si>
-    <t>in_TradSheetName</t>
-  </si>
-  <si>
     <t>Hoja 1</t>
   </si>
   <si>
@@ -88,72 +78,30 @@
     <t>rpanotificaciones@tecnoyar.com</t>
   </si>
   <si>
-    <t>TempSheetName</t>
-  </si>
-  <si>
     <t>GmailID</t>
   </si>
   <si>
     <t>GmailPass</t>
   </si>
   <si>
-    <t>NO_SOCIOS_BD_Argentina__Semana_</t>
-  </si>
-  <si>
     <t>notificacionesrpa.tecnoyar@gmail.com</t>
   </si>
   <si>
     <t>Rp4.C1n3p0l1s</t>
   </si>
   <si>
-    <t>PartnerTempBDPath</t>
-  </si>
-  <si>
-    <t>NonPartnerTempBDPath</t>
-  </si>
-  <si>
     <t>InputnonPartnerFilePath</t>
   </si>
   <si>
-    <t>InputPartnerFilePath</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Base de Datos/Socios</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/30 Envio Semana 30/Argentina/Tradicional/Socios</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS 2021/1 Directorio</t>
   </si>
   <si>
-    <t>input file path for partner file</t>
-  </si>
-  <si>
     <t>input file path for non partner file</t>
   </si>
   <si>
-    <t>TempPartnerSheetName</t>
-  </si>
-  <si>
-    <t>SOCIOS_BD_Argentina_Semana_Sema</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos</t>
-  </si>
-  <si>
     <t>BD_ENCUESTA_LARGA_GULF_Tradicio</t>
   </si>
   <si>
-    <t xml:space="preserve"> /Planeacion/0.Envios TS 2021/0 Envios 0/GULF/TRADICIONAL</t>
-  </si>
-  <si>
-    <t>SurvayFileTraditionalPath</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS 2021/0 Envios 0/GULF/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>BDVIPfilePath</t>
   </si>
   <si>
@@ -163,9 +111,6 @@
     <t>InputSheetName</t>
   </si>
   <si>
-    <t>Transaction</t>
-  </si>
-  <si>
     <t>InputSheetNewName</t>
   </si>
   <si>
@@ -209,6 +154,24 @@
   </si>
   <si>
     <t>DirectirioSheetName</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/BD Consolidada</t>
+  </si>
+  <si>
+    <t>REPORTE_ESTUDIOC_ESPANIA_46</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS 2021/33 Envio Semana 31/ESPAÑA/BD Consolidada/Exportada</t>
+  </si>
+  <si>
+    <t>DirectorioFilePath</t>
+  </si>
+  <si>
+    <t>DirectorioSheetName</t>
+  </si>
+  <si>
+    <t>España</t>
   </si>
 </sst>
 </file>
@@ -358,14 +321,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -387,15 +347,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -721,18 +672,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="21"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="16">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75">
+      <c r="A29" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75">
+      <c r="A30" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B25" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Z978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="72" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41" customWidth="1"/>
+    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -740,7 +908,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -770,1388 +938,6 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A17" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A18" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A19" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{FF7F0B36-CE90-4A91-B3A6-3587652CB510}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C27"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
-      <c r="A4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15.75">
-      <c r="A5" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75">
-      <c r="A7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75">
-      <c r="A15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75">
-      <c r="A18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B25" r:id="rId1" xr:uid="{58EC0946-E8B4-4BDB-80EA-7ED2F2D369BC}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z978"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
     <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
@@ -2165,29 +951,29 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>26</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B5" s="14"/>
+      <c r="B5" s="13"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3166,7 +1952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
@@ -3228,17 +2014,17 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="10"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="6"/>
-      <c r="B13" s="13"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="12"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -3248,22 +2034,22 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B19" s="11"/>
+      <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="15"/>
+      <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
updated input file manipulation and applied log messages
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisSpain\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A68F230-5310-4E65-B764-0428C0D60D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3F4EC2-39BE-45F8-B68A-710446E2AD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -899,7 +899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1976,7 +1976,7 @@
   <dimension ref="A1:Z1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
files updated after testing
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisSpain\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3F4EC2-39BE-45F8-B68A-710446E2AD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18BE632-36E9-4EA5-B6EC-2011A761960D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -159,19 +159,37 @@
     <t>manindersinghbisht77@gmail.com</t>
   </si>
   <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ESPAÑA/Base de Datos</t>
-  </si>
-  <si>
-    <t>REPORTE_ESTUDIOC_ESPANIA_03_202</t>
-  </si>
-  <si>
-    <t>/Planeacion/0.Envios TS/2022/04 Envio Semana 04/ESPAÑA/Base de Datos/Exportadas</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
   </si>
   <si>
     <t>ToCC</t>
+  </si>
+  <si>
+    <t>REPORTE_ESTUDIOC_ESPANIA_04_202</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/ESPAÑA/BD Consolidada</t>
+  </si>
+  <si>
+    <t>Key Word</t>
+  </si>
+  <si>
+    <t>REPORTE, ESTUDIOC, ESPANIA</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/ESPAÑA/LUXURY</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/ESPAÑA/TRADICIONAL</t>
+  </si>
+  <si>
+    <t>Path luxury File when it is divide</t>
+  </si>
+  <si>
+    <t>Path for Traditional File when it is divide</t>
+  </si>
+  <si>
+    <t>/Planeacion/0.Envios TS/2022/05 Envio Semana 05/ESPAÑA/BD Consolidada/Exportadas</t>
   </si>
 </sst>
 </file>
@@ -675,19 +693,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:5" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,27 +716,33 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75">
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="E2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -725,7 +750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75">
+    <row r="5" spans="1:5" ht="15.75">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -733,50 +758,57 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75">
+    <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="2"/>
       <c r="B6" s="20"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75">
+    <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="20"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="21"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75">
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="20"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75">
+    <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -784,12 +816,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75">
+    <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -805,7 +837,7 @@
         <v>35</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -824,7 +856,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -875,7 +907,7 @@
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75">
@@ -982,7 +1014,7 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
config file is updated
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48EC985-FDD2-47E3-A1C3-8FA84647D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DC4FD-1998-4888-BF0D-9C9796F6E2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -153,18 +153,9 @@
     <t>BDTempFileName</t>
   </si>
   <si>
-    <t>Tomail</t>
-  </si>
-  <si>
-    <t>manindersinghbisht77@gmail.com</t>
-  </si>
-  <si>
     <t>/Planeacion/0.Envios TS/1 Directorio</t>
   </si>
   <si>
-    <t>ToCC</t>
-  </si>
-  <si>
     <t>REPORTE_ESTUDIOC_ESPANIA_04_202</t>
   </si>
   <si>
@@ -199,13 +190,105 @@
   </si>
   <si>
     <t>WorkingEndDate</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- Data doesn't belong to this week</t>
+  </si>
+  <si>
+    <t>DataNoBelongToCurrentWeekMailBody</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+Please find the below data which does not belong to current week.&lt;br/&gt;
+[Nothisweekdatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>MailTo</t>
+  </si>
+  <si>
+    <t>rhernandez@tecnoyar.com.mx;arerodriguez@tecnoyar.com</t>
+  </si>
+  <si>
+    <t>MailCC</t>
+  </si>
+  <si>
+    <t>arerodriguez@tecnoyar.com</t>
+  </si>
+  <si>
+    <t>InputFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Error- Input file Notification</t>
+  </si>
+  <si>
+    <t>InputFileExceptionbody</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionSubject</t>
+  </si>
+  <si>
+    <t>Notification- Not All file Got downloaded</t>
+  </si>
+  <si>
+    <t>downloadFileExceptionbody</t>
+  </si>
+  <si>
+    <t>WrongNameMailSubject</t>
+  </si>
+  <si>
+    <t>Notification- name is not correct</t>
+  </si>
+  <si>
+    <t>WrongNameMailbody</t>
+  </si>
+  <si>
+    <t>NADirectrioMailSubject</t>
+  </si>
+  <si>
+    <t>NADirectrioMailBody</t>
+  </si>
+  <si>
+    <t>#NA data found at input file in "N" column</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepolish USA run, below is the detail of error&lt;br/&gt;
+[error]&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+There is a error in Cinepos USA process run, below is the detail of error&lt;br/&gt;
+Not all required files got downloaded from FTP&lt;br/&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>Dear Team&lt;br/&gt;
+below names are not correct in USA  process input file.&lt;br/&gt;
+[wrongnamedatatable]&lt;br&gt;
+Also let us know if anything is required&lt;br/&gt;
+Thank you,&lt;br/&gt;
+**********************This is system generated E-Mail, please do not respond on this************</t>
+  </si>
+  <si>
+    <t>file of the USA mark contains errors in the "N" column called "clave_tipo_cine"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -321,12 +404,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -345,17 +422,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -366,7 +439,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -386,13 +458,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -722,28 +803,28 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="20" t="s">
-        <v>48</v>
+      <c r="B2" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -751,14 +832,14 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -766,30 +847,30 @@
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="2"/>
-      <c r="B6" s="20"/>
+      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>51</v>
+      <c r="B7" s="18" t="s">
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="19"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
@@ -800,11 +881,11 @@
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>52</v>
+      <c r="B10" s="18" t="s">
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -816,15 +897,15 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="20" t="s">
-        <v>48</v>
+      <c r="B13" s="18" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="15" t="s">
         <v>14</v>
       </c>
     </row>
@@ -832,8 +913,8 @@
       <c r="A16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>55</v>
+      <c r="B16" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -848,8 +929,8 @@
       <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>55</v>
+      <c r="B19" s="18" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -868,7 +949,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -886,7 +967,7 @@
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>21</v>
       </c>
     </row>
@@ -894,7 +975,7 @@
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -902,28 +983,28 @@
       <c r="A27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="18" t="s">
         <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="18" t="s">
         <v>40</v>
       </c>
       <c r="B31" t="s">
@@ -943,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -990,93 +1071,214 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="20">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="25" t="s">
         <v>20</v>
       </c>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="25" t="s">
         <v>21</v>
       </c>
+      <c r="C4" s="20"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>44</v>
-      </c>
+      <c r="A5" s="20"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="20"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="2"/>
+      <c r="A7" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="24">
+      <c r="A8" s="20"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="20"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="20"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="20"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="20"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="20"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="20"/>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="20"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="20"/>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="20"/>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="20"/>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="21">
         <v>44578</v>
       </c>
-      <c r="C8" s="24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="24">
+      <c r="C24" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="21">
         <v>44584</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+      <c r="C25" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -2025,11 +2227,8 @@
     <row r="978" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{E9BA6301-C831-40FC-B441-2526FBE4C1AA}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2095,17 +2294,17 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="C11" s="9"/>
+      <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2"/>
@@ -2115,22 +2314,22 @@
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B19" s="10"/>
+      <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B20" s="11"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B21" s="13"/>
+      <c r="B21" s="12"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
first round of testing done.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazmin\AutomationProcesses\cinepolis\CinepolishSpain\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yazmin\Documents\UiPath\CinepolisSpain\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8DC4FD-1998-4888-BF0D-9C9796F6E2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6AB1CA2-CE29-4F01-9FAF-ED0326B205CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="4" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <t>MailTo</t>
   </si>
   <si>
-    <t>rhernandez@tecnoyar.com.mx;arerodriguez@tecnoyar.com</t>
-  </si>
-  <si>
     <t>MailCC</t>
   </si>
   <si>
@@ -282,6 +279,9 @@
   </si>
   <si>
     <t>file of the USA mark contains errors in the "N" column called "clave_tipo_cine"</t>
+  </si>
+  <si>
+    <t>rhernandez@tecnoyar.com.mx</t>
   </si>
 </sst>
 </file>
@@ -788,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D20D9A4-B24A-48FB-83BA-8E4507ED59B9}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -851,9 +851,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75">
+    <row r="6" spans="1:5">
       <c r="A6" s="2"/>
-      <c r="B6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="15.75">
       <c r="A7" s="2" t="s">
@@ -1024,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z978"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1132,16 +1131,16 @@
         <v>60</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>62</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>63</v>
       </c>
       <c r="C10" s="20"/>
     </row>
@@ -1152,19 +1151,19 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="20"/>
     </row>
@@ -1175,19 +1174,19 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>68</v>
       </c>
       <c r="C15" s="20"/>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="20"/>
     </row>
@@ -1198,19 +1197,19 @@
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>71</v>
       </c>
       <c r="C18" s="20"/>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C19" s="20"/>
     </row>
@@ -1221,19 +1220,19 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C21" s="20"/>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>74</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>75</v>
       </c>
       <c r="C22" s="20"/>
     </row>
@@ -1247,7 +1246,7 @@
         <v>53</v>
       </c>
       <c r="B24" s="21">
-        <v>44578</v>
+        <v>44585</v>
       </c>
       <c r="C24" s="21" t="s">
         <v>54</v>
@@ -1258,7 +1257,7 @@
         <v>55</v>
       </c>
       <c r="B25" s="21">
-        <v>44584</v>
+        <v>44591</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>54</v>

</xml_diff>